<commit_message>
Refactored abrvs into its own module
</commit_message>
<xml_diff>
--- a/data/test/test_gpt3F_entsF.xlsx
+++ b/data/test/test_gpt3F_entsF.xlsx
@@ -527,12 +527,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>[{"factor": ["serum", "thioredoxin concentration"], "outcome": ["in-hospital major adverse event"]}, {"factor": ["admission", "glasgow coma scale score"], "outcome": ["in-hospital major adverse event"]}]</t>
+          <t>[{"factor": ["thioredoxin concentration", "serum"], "outcome": ["in-hospital major adverse event"]}, {"factor": ["glasgow coma scale score", "admission"], "outcome": ["in-hospital major adverse event"]}]</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>[{"factor": ["thioredoxin concentration"], "outcome": ["imaes"]}, {"factor": ["admission", "glasgow coma scale score"], "outcome": ["imaes"]}]</t>
+          <t>[{"factor": ["thioredoxin concentration"], "outcome": ["imaes"]}, {"factor": ["glasgow coma scale score", "admission"], "outcome": ["imaes"]}]</t>
         </is>
       </c>
     </row>
@@ -649,12 +649,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>[{"factor": ["mif", "macrophage migration inhibitory factor"], "outcome": ["clinical outcome", "trauma", "inflammation", "severity"]}]</t>
+          <t>[{"factor": ["mif", "macrophage migration inhibitory factor"], "outcome": ["severity", "inflammation", "clinical outcome", "trauma"]}]</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>[{"factor": ["mif", "macrophage migration inhibitory factor"], "outcome": ["unspecified clinical outcome", "inflammation", "severity"]}]</t>
+          <t>[{"factor": ["mif", "macrophage migration inhibitory factor"], "outcome": ["severity", "inflammation", "unspecified clinical outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -710,12 +710,12 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>[{"factor": ["glasgow coma scale score"], "outcome": ["gos", "glasgow outcome scale"]}, {"factor": ["artificial ventilation"], "outcome": ["mortality rate"]}, {"factor": ["monitoring", "intracranial"], "outcome": ["good", "outcome", "long-term"]}]</t>
+          <t>[{"factor": ["glasgow coma scale score"], "outcome": ["glasgow outcome scale", "gos"]}, {"factor": ["artificial ventilation"], "outcome": ["mortality rate"]}, {"factor": ["monitoring", "intracranial"], "outcome": ["outcome", "long-term", "good"]}]</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[{"factor": ["glasgow coma scale score"], "outcome": ["gos"]}, {"factor": ["artificial ventilation"], "outcome": ["mortality"]}, {"factor": ["monitoring", "intracranial"], "outcome": ["unspecified clinical outcome", "long-term"]}]</t>
+          <t>[{"factor": ["glasgow coma scale score"], "outcome": ["gos"]}, {"factor": ["artificial ventilation"], "outcome": ["mortality"]}, {"factor": ["monitoring", "intracranial"], "outcome": ["long-term", "unspecified clinical outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -771,12 +771,12 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>[{"factor": ["calculator", "impact", "prognosis"], "outcome": ["severe", "patient", "elderly", "tbi", "outcome"]}, {"factor": ["outcome", "fatal", "expect risk"], "outcome": ["conservative treatment", "risk"]}, {"factor": ["unfavorable", "outcome", "predict risk"], "outcome": ["actual", "unfavorable", "predict", "rate", "outcome", "risk"]}]</t>
+          <t>[{"factor": ["impact", "calculator", "prognosis"], "outcome": ["patient", "elderly", "severe", "outcome", "tbi"]}, {"factor": ["expect risk", "fatal", "outcome"], "outcome": ["risk", "conservative treatment"]}, {"factor": ["outcome", "unfavorable", "predict risk"], "outcome": ["actual", "rate", "risk", "outcome", "unfavorable", "predict"]}]</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>[{"factor": ["calculator", "impact model"], "outcome": ["unspecified clinical outcome", "elderly"]}, {"factor": ["fatal", "expect risk"], "outcome": ["conservative treatment"]}, {"factor": ["predict risk"], "outcome": ["actual", "unspecified clinical outcome", "predict"]}]</t>
+          <t>[{"factor": ["calculator", "impact model"], "outcome": ["elderly", "unspecified clinical outcome"]}, {"factor": ["expect risk", "fatal"], "outcome": ["conservative treatment"]}, {"factor": ["predict risk"], "outcome": ["predict", "actual", "unspecified clinical outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>[{"factor": ["compute tomography", "ct"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["marshall and rotterdam scoring system"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["basal cistern absence"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["positive midline shift"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["hemorrhagic mass volume"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["intraventricular", "subarachnoid hemorrhage"], "outcome": ["patient", "tbi", "death"]}]</t>
+          <t>[{"factor": ["compute tomography", "ct"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["marshall and rotterdam scoring system"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["basal cistern absence"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["positive midline shift"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["hemorrhagic mass volume"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["intraventricular", "subarachnoid hemorrhage"], "outcome": ["death", "patient", "tbi"]}]</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -954,12 +954,12 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>[{"factor": ["apache ii"], "outcome": ["icu-treated", "patient", "mortality", "six-month", "tbi"]}, {"factor": ["sap ii"], "outcome": ["icu-treated", "patient", "mortality", "six-month", "tbi"]}, {"factor": ["sofa"], "outcome": ["icu-treated", "patient", "mortality", "six-month", "tbi"]}, {"factor": ["age"], "outcome": ["icu-treated", "patient", "mortality", "six-month", "tbi"]}, {"factor": ["glasgow coma scale"], "outcome": ["icu-treated", "patient", "mortality", "six-month", "tbi"]}]</t>
+          <t>[{"factor": ["apache ii"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["sap ii"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["sofa"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["age"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["glasgow coma scale"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}]</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>[{"factor": ["apache ii"], "outcome": ["mortality", "six-month", "icu-treated"]}, {"factor": ["sap ii"], "outcome": ["mortality", "six-month", "icu-treated"]}, {"factor": ["sofa"], "outcome": ["mortality", "six-month", "icu-treated"]}, {"factor": ["age"], "outcome": ["mortality", "six-month", "icu-treated"]}, {"factor": ["gcs"], "outcome": ["mortality", "six-month", "icu-treated"]}]</t>
+          <t>[{"factor": ["apache ii"], "outcome": ["mortality", "icu-treated", "six-month"]}, {"factor": ["sap ii"], "outcome": ["mortality", "icu-treated", "six-month"]}, {"factor": ["sofa"], "outcome": ["mortality", "icu-treated", "six-month"]}, {"factor": ["age"], "outcome": ["mortality", "icu-treated", "six-month"]}, {"factor": ["gcs"], "outcome": ["mortality", "icu-treated", "six-month"]}]</t>
         </is>
       </c>
     </row>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>[{"factor": ["v/c ratio"], "outcome": ["lcf score", "drs", "gos score"]}]</t>
+          <t>[{"factor": ["v/c ratio"], "outcome": ["drs", "gos score", "lcf score"]}]</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>[{"factor": ["timp-1 level", "serum"], "outcome": ["patient", "mortality", "severe", "tbi"]}]</t>
+          <t>[{"factor": ["timp-1 level", "serum"], "outcome": ["tbi", "patient", "severe", "mortality"]}]</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1137,12 +1137,12 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>[{"factor": ["mri", "contusion", "evidence"], "outcome": ["glasgow outcome scale-extended", "gos-e"]}, {"factor": ["fa", "severely", "reduce", "roi"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["age"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}, {"factor": ["fa", "severely", "reduce", "roi"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}]</t>
+          <t>[{"factor": ["evidence", "contusion", "mri"], "outcome": ["glasgow outcome scale-extended", "gos-e"]}, {"factor": ["roi", "severely", "fa", "reduce"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["age"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}, {"factor": ["roi", "severely", "fa", "reduce"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}]</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>[{"factor": ["mri", "contusion", "evidence"], "outcome": ["gos-e"]}, {"factor": ["fa", "reduce", "roi", "severely"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["age"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}, {"factor": ["fa", "reduce", "roi", "severely"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}]</t>
+          <t>[{"factor": ["evidence", "contusion", "mri"], "outcome": ["gos-e"]}, {"factor": ["roi", "severely", "fa", "reduce"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["age"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}, {"factor": ["roi", "severely", "fa", "reduce"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}]</t>
         </is>
       </c>
     </row>
@@ -1198,12 +1198,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>[{"factor": ["preinjury", "depressive symptom"], "outcome": ["health-related quality-of-life", "cognitive", "affective/behavioral", "physical problem"]}]</t>
+          <t>[{"factor": ["preinjury", "depressive symptom"], "outcome": ["affective/behavioral", "physical problem", "cognitive", "health-related quality-of-life"]}]</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>[{"factor": ["preinjury", "depressive symptom"], "outcome": ["health-related quality-of-life", "cognitive", "affective/behavioral", "physical problem"]}]</t>
+          <t>[{"factor": ["preinjury", "depressive symptom"], "outcome": ["affective/behavioral", "physical problem", "cognitive", "health-related quality-of-life"]}]</t>
         </is>
       </c>
     </row>
@@ -1320,12 +1320,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>[{"factor": ["age"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["sex"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["deyo-charlson comorbidity index", "score"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["hospital volume"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["volume", "surgeon"], "outcome": ["in-hospital mortality rate"]}]</t>
+          <t>[{"factor": ["age"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["sex"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["score", "deyo-charlson comorbidity index"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["hospital volume"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["surgeon", "volume"], "outcome": ["in-hospital mortality rate"]}]</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>[{"factor": ["age"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["sex"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["deyo-charlson comorbidity index"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["hospital volume"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["volume", "surgeon"], "outcome": ["in-hospital mortality rate"]}]</t>
+          <t>[{"factor": ["age"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["sex"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["deyo-charlson comorbidity index"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["hospital volume"], "outcome": ["in-hospital mortality rate"]}, {"factor": ["surgeon", "volume"], "outcome": ["in-hospital mortality rate"]}]</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>[{"factor": ["age"], "outcome": ["icu", "risk"]}, {"factor": ["gender"], "outcome": ["icu", "risk"]}, {"factor": ["etiology", "injury"], "outcome": ["icu", "risk"]}]</t>
+          <t>[{"factor": ["age"], "outcome": ["risk", "icu"]}, {"factor": ["gender"], "outcome": ["risk", "icu"]}, {"factor": ["etiology", "injury"], "outcome": ["risk", "icu"]}]</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1442,12 +1442,12 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>[{"factor": ["csf", "cerebrospinal fluid", "concentration", "amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["concentration", "plasma", "amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["csf", "change", "abeta42", "concentration"], "outcome": ["neurological status"]}]</t>
+          <t>[{"factor": ["concentration", "cerebrospinal fluid", "csf", "amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["concentration", "plasma", "amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["abeta42", "change", "concentration", "csf"], "outcome": ["neurological status"]}]</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>[{"factor": ["amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["change", "abeta42"], "outcome": ["neurological status"]}]</t>
+          <t>[{"factor": ["amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["abeta42", "change"], "outcome": ["neurological status"]}]</t>
         </is>
       </c>
     </row>
@@ -1503,12 +1503,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>[{"factor": ["plasminogen activator receptor", "urokinase", "supar", "soluble"], "outcome": ["tbi", "traumatic brain injury"]}, {"factor": ["glasgow coma scale", "score"], "outcome": ["tbi", "severity"]}, {"factor": ["d-dimer"], "outcome": ["tbi", "mortality", "patient"]}]</t>
+          <t>[{"factor": ["plasminogen activator receptor", "supar", "soluble", "urokinase"], "outcome": ["traumatic brain injury", "tbi"]}, {"factor": ["glasgow coma scale", "score"], "outcome": ["severity", "tbi"]}, {"factor": ["d-dimer"], "outcome": ["tbi", "patient", "mortality"]}]</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[{"factor": ["plasminogen activator receptor", "urokinase", "supar", "soluble"], "outcome": []}, {"factor": ["gcs"], "outcome": ["severity"]}, {"factor": ["d-dimer"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": ["soluble", "plasminogen activator receptor", "supar", "urokinase"], "outcome": []}, {"factor": ["gcs"], "outcome": ["severity"]}, {"factor": ["d-dimer"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -1564,12 +1564,12 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>[{"factor": ["motor score", "gcs"], "outcome": ["mortality", "month"]}, {"factor": ["age"], "outcome": ["mortality", "month"]}, {"factor": ["sex"], "outcome": ["mortality", "month"]}, {"factor": ["injury", "mechanism"], "outcome": ["mortality", "month"]}, {"factor": ["glasgow coma scale"], "outcome": ["mortality", "month"]}, {"factor": ["intubation"], "outcome": ["mortality", "month"]}, {"factor": ["pupil"], "outcome": ["mortality", "month"]}, {"factor": ["systolic blood pressure"], "outcome": ["mortality", "month"]}, {"factor": ["respiratory rate"], "outcome": ["mortality", "month"]}, {"factor": ["body temperature"], "outcome": ["mortality", "month"]}, {"factor": ["ph", "arterial"], "outcome": ["mortality", "month"]}, {"factor": ["arterial partial pressure", "carbon dioxide"], "outcome": ["mortality", "month"]}, {"factor": ["arterial partial pressure"], "outcome": ["mortality", "month"]}, {"factor": ["serum sodium"], "outcome": ["mortality", "month"]}, {"factor": ["serum potassium"], "outcome": ["mortality", "month"]}, {"factor": ["serum chloride"], "outcome": ["mortality", "month"]}, {"factor": ["serum calcium"], "outcome": ["mortality", "month"]}, {"factor": ["serum glucose"], "outcome": ["mortality", "month"]}, {"factor": ["urea nitrogen"], "outcome": ["mortality", "month"]}, {"factor": ["creatinine"], "outcome": ["mortality", "month"]}, {"factor": ["international", "ratio"], "outcome": ["mortality", "month"]}]</t>
+          <t>[{"factor": ["motor score", "gcs"], "outcome": ["month", "mortality"]}, {"factor": ["age"], "outcome": ["month", "mortality"]}, {"factor": ["sex"], "outcome": ["month", "mortality"]}, {"factor": ["injury", "mechanism"], "outcome": ["month", "mortality"]}, {"factor": ["glasgow coma scale"], "outcome": ["month", "mortality"]}, {"factor": ["intubation"], "outcome": ["month", "mortality"]}, {"factor": ["pupil"], "outcome": ["month", "mortality"]}, {"factor": ["systolic blood pressure"], "outcome": ["month", "mortality"]}, {"factor": ["respiratory rate"], "outcome": ["month", "mortality"]}, {"factor": ["body temperature"], "outcome": ["month", "mortality"]}, {"factor": ["arterial", "ph"], "outcome": ["month", "mortality"]}, {"factor": ["arterial partial pressure", "carbon dioxide"], "outcome": ["month", "mortality"]}, {"factor": ["arterial partial pressure"], "outcome": ["month", "mortality"]}, {"factor": ["serum sodium"], "outcome": ["month", "mortality"]}, {"factor": ["serum potassium"], "outcome": ["month", "mortality"]}, {"factor": ["serum chloride"], "outcome": ["month", "mortality"]}, {"factor": ["serum calcium"], "outcome": ["month", "mortality"]}, {"factor": ["serum glucose"], "outcome": ["month", "mortality"]}, {"factor": ["urea nitrogen"], "outcome": ["month", "mortality"]}, {"factor": ["creatinine"], "outcome": ["month", "mortality"]}, {"factor": ["ratio", "international"], "outcome": ["month", "mortality"]}]</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>[{"factor": ["motor score", "gcs"], "outcome": ["mortality"]}, {"factor": ["age"], "outcome": ["mortality"]}, {"factor": ["sex"], "outcome": ["mortality"]}, {"factor": ["mechanism"], "outcome": ["mortality"]}, {"factor": ["gcs"], "outcome": ["mortality"]}, {"factor": ["intubation"], "outcome": ["mortality"]}, {"factor": ["pupil"], "outcome": ["mortality"]}, {"factor": ["sbp"], "outcome": ["mortality"]}, {"factor": ["respiratory rate"], "outcome": ["mortality"]}, {"factor": ["body temperature"], "outcome": ["mortality"]}, {"factor": ["ph", "arterial"], "outcome": ["mortality"]}, {"factor": ["arterial partial pressure", "carbon dioxide"], "outcome": ["mortality"]}, {"factor": ["arterial partial pressure"], "outcome": ["mortality"]}, {"factor": ["serum sodium"], "outcome": ["mortality"]}, {"factor": ["serum potassium"], "outcome": ["mortality"]}, {"factor": ["serum chloride"], "outcome": ["mortality"]}, {"factor": ["serum calcium"], "outcome": ["mortality"]}, {"factor": ["serum glucose"], "outcome": ["mortality"]}, {"factor": ["urea nitrogen"], "outcome": ["mortality"]}, {"factor": ["creatinine"], "outcome": ["mortality"]}, {"factor": ["international"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": ["motor score", "gcs"], "outcome": ["mortality"]}, {"factor": ["age"], "outcome": ["mortality"]}, {"factor": ["sex"], "outcome": ["mortality"]}, {"factor": ["mechanism"], "outcome": ["mortality"]}, {"factor": ["gcs"], "outcome": ["mortality"]}, {"factor": ["intubation"], "outcome": ["mortality"]}, {"factor": ["pupil"], "outcome": ["mortality"]}, {"factor": ["sbp"], "outcome": ["mortality"]}, {"factor": ["respiratory rate"], "outcome": ["mortality"]}, {"factor": ["body temperature"], "outcome": ["mortality"]}, {"factor": ["arterial", "ph"], "outcome": ["mortality"]}, {"factor": ["arterial partial pressure", "carbon dioxide"], "outcome": ["mortality"]}, {"factor": ["arterial partial pressure"], "outcome": ["mortality"]}, {"factor": ["serum sodium"], "outcome": ["mortality"]}, {"factor": ["serum potassium"], "outcome": ["mortality"]}, {"factor": ["serum chloride"], "outcome": ["mortality"]}, {"factor": ["serum calcium"], "outcome": ["mortality"]}, {"factor": ["serum glucose"], "outcome": ["mortality"]}, {"factor": ["urea nitrogen"], "outcome": ["mortality"]}, {"factor": ["creatinine"], "outcome": ["mortality"]}, {"factor": ["international"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>[{"factor": ["cct", "central conduction time"], "outcome": ["unspecified clinical outcome", "long-term"]}, {"factor": ["latency"], "outcome": ["unspecified clinical outcome", "long-term"]}]</t>
+          <t>[{"factor": ["cct", "central conduction time"], "outcome": ["long-term", "unspecified clinical outcome"]}, {"factor": ["latency"], "outcome": ["long-term", "unspecified clinical outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -1747,7 +1747,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>[{"factor": ["sbp", "systolic blood pressure"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": ["systolic blood pressure", "sbp"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1869,12 +1869,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>[{"factor": ["tsp-1"], "outcome": ["unfavorable", "mortality", "outcome", "1-week"]}]</t>
+          <t>[{"factor": ["tsp-1"], "outcome": ["outcome", "unfavorable", "1-week", "mortality"]}]</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>[{"factor": ["tsp-1"], "outcome": ["mortality", "unspecified clinical outcome", "1-week"]}]</t>
+          <t>[{"factor": ["tsp-1"], "outcome": ["1-week", "unspecified clinical outcome", "mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -1930,12 +1930,12 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>[{"factor": ["brain-derived neurotrophic factor (bdnf)", "plasma level"], "outcome": ["severe", "patient", "intensive care unit", "mortality", "icu", "tbi"]}]</t>
+          <t>[{"factor": ["brain-derived neurotrophic factor (bdnf)", "plasma level"], "outcome": ["icu", "mortality", "patient", "severe", "intensive care unit", "tbi"]}]</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>[{"factor": ["brain-derived neurotrophic factor (bdnf)", "plasma level"], "outcome": ["mortality", "icu"]}]</t>
+          <t>[{"factor": ["brain-derived neurotrophic factor (bdnf)", "plasma level"], "outcome": ["icu", "mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -1991,12 +1991,12 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>[{"factor": ["crash-ct model"], "outcome": ["days", "death"]}, {"factor": ["age"], "outcome": ["older", "model", "performance", "patient"]}, {"factor": ["glasgow coma scale score"], "outcome": ["model", "discrimination"]}, {"factor": ["hosmer-lemeshow p value"], "outcome": ["model", "calibration"]}]</t>
+          <t>[{"factor": ["crash-ct model"], "outcome": ["death", "days"]}, {"factor": ["age"], "outcome": ["patient", "performance", "model", "older"]}, {"factor": ["glasgow coma scale score"], "outcome": ["discrimination", "model"]}, {"factor": ["hosmer-lemeshow p value"], "outcome": ["calibration", "model"]}]</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>[{"factor": ["crash-ct model"], "outcome": ["mortality"]}, {"factor": ["age"], "outcome": ["older", "model", "performance"]}, {"factor": ["glasgow coma scale score"], "outcome": ["model", "discrimination"]}, {"factor": ["hosmer-lemeshow p value"], "outcome": ["model", "calibration"]}]</t>
+          <t>[{"factor": ["crash-ct model"], "outcome": ["mortality"]}, {"factor": ["age"], "outcome": ["performance", "model", "older"]}, {"factor": ["glasgow coma scale score"], "outcome": ["discrimination", "model"]}, {"factor": ["hosmer-lemeshow p value"], "outcome": ["calibration", "model"]}]</t>
         </is>
       </c>
     </row>
@@ -2052,12 +2052,12 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>[{"factor": ["time to death"], "outcome": ["life-sustaining", "withdrawal", "therapy"]}, {"factor": ["glasgow coma scale", "score"], "outcome": ["mortality"]}, {"factor": ["ais", "head abbreviate injury scale", "score"], "outcome": ["mortality"]}, {"factor": ["comorbiditie", "multiple"], "outcome": ["mortality"]}, {"factor": ["traumatic", "subarachnoid hemorrhage"], "outcome": ["mortality"]}, {"factor": ["intracerebral mass lesion"], "outcome": ["mortality"]}, {"factor": ["brainstem lesion"], "outcome": ["mortality"]}, {"factor": ["basal cistern", "absent", "sign of compress"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": ["time to death"], "outcome": ["withdrawal", "life-sustaining", "therapy"]}, {"factor": ["glasgow coma scale", "score"], "outcome": ["mortality"]}, {"factor": ["score", "ais", "head abbreviate injury scale"], "outcome": ["mortality"]}, {"factor": ["comorbiditie", "multiple"], "outcome": ["mortality"]}, {"factor": ["subarachnoid hemorrhage", "traumatic"], "outcome": ["mortality"]}, {"factor": ["intracerebral mass lesion"], "outcome": ["mortality"]}, {"factor": ["brainstem lesion"], "outcome": ["mortality"]}, {"factor": ["absent", "sign of compress", "basal cistern"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[{"factor": ["time to death"], "outcome": ["life-sustaining", "withdrawal", "therapy"]}, {"factor": ["gcs"], "outcome": ["mortality"]}, {"factor": ["ais", "head abbreviate injury scale"], "outcome": ["mortality"]}, {"factor": ["comorbiditie", "multiple"], "outcome": ["mortality"]}, {"factor": ["subarachnoid hemorrhage"], "outcome": ["mortality"]}, {"factor": ["intracerebral mass lesion"], "outcome": ["mortality"]}, {"factor": ["brainstem lesion"], "outcome": ["mortality"]}, {"factor": ["basal cistern", "absent", "sign of compress"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": ["time to death"], "outcome": ["withdrawal", "life-sustaining", "therapy"]}, {"factor": ["gcs"], "outcome": ["mortality"]}, {"factor": ["ais", "head abbreviate injury scale"], "outcome": ["mortality"]}, {"factor": ["comorbiditie", "multiple"], "outcome": ["mortality"]}, {"factor": ["subarachnoid hemorrhage"], "outcome": ["mortality"]}, {"factor": ["intracerebral mass lesion"], "outcome": ["mortality"]}, {"factor": ["brainstem lesion"], "outcome": ["mortality"]}, {"factor": ["absent", "sign of compress", "basal cistern"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>[{"factor": ["core model"], "outcome": ["mortality"]}, {"factor": ["extend model"], "outcome": ["mortality"]}, {"factor": ["lab model"], "outcome": ["mortality"]}, {"factor": ["core model"], "outcome": ["unfavorable", "outcome"]}, {"factor": ["extend model"], "outcome": ["unfavorable", "outcome"]}, {"factor": ["lab model"], "outcome": ["unfavorable", "outcome"]}]</t>
+          <t>[{"factor": ["core model"], "outcome": ["mortality"]}, {"factor": ["extend model"], "outcome": ["mortality"]}, {"factor": ["lab model"], "outcome": ["mortality"]}, {"factor": ["core model"], "outcome": ["outcome", "unfavorable"]}, {"factor": ["extend model"], "outcome": ["outcome", "unfavorable"]}, {"factor": ["lab model"], "outcome": ["outcome", "unfavorable"]}]</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -2174,12 +2174,12 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>[{"factor": ["glasgow coma scale", "score"], "outcome": ["unfavorable", "mortality", "outcome", "1-week"]}]</t>
+          <t>[{"factor": ["glasgow coma scale", "score"], "outcome": ["outcome", "unfavorable", "1-week", "mortality"]}]</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>[{"factor": ["gcs"], "outcome": ["mortality", "unspecified clinical outcome", "1-week"]}]</t>
+          <t>[{"factor": ["gcs"], "outcome": ["1-week", "unspecified clinical outcome", "mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -2235,7 +2235,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>[{"factor": ["gcs", "glasgow coma scale"], "outcome": ["tbi", "severity"]}, {"factor": ["post-traumatic amnesia", "pta", "duration"], "outcome": ["tbi", "olfactory problem"]}]</t>
+          <t>[{"factor": ["gcs", "glasgow coma scale"], "outcome": ["severity", "tbi"]}, {"factor": ["pta", "duration", "post-traumatic amnesia"], "outcome": ["olfactory problem", "tbi"]}]</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>[{"factor": ["level", "il-6"], "outcome": ["septic", "development"]}, {"factor": ["c-reactive protein level"], "outcome": ["development", "multiple organ dysfunction"]}]</t>
+          <t>[{"factor": ["level", "il-6"], "outcome": ["septic", "development"]}, {"factor": ["c-reactive protein level"], "outcome": ["multiple organ dysfunction", "development"]}]</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2357,12 +2357,12 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>[{"factor": ["rotterdam"], "outcome": ["weeks", "hospital discharge", "death"]}, {"factor": ["age"], "outcome": ["weeks", "hospital discharge", "death"]}, {"factor": ["sex"], "outcome": ["weeks", "hospital discharge", "death"]}, {"factor": ["glasgow coma scale score"], "outcome": ["weeks", "hospital discharge", "death"]}]</t>
+          <t>[{"factor": ["rotterdam"], "outcome": ["death", "hospital discharge", "weeks"]}, {"factor": ["age"], "outcome": ["death", "hospital discharge", "weeks"]}, {"factor": ["sex"], "outcome": ["death", "hospital discharge", "weeks"]}, {"factor": ["glasgow coma scale score"], "outcome": ["death", "hospital discharge", "weeks"]}]</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>[{"factor": ["rotterdam"], "outcome": ["mortality", "hospital discharge"]}, {"factor": ["age"], "outcome": ["mortality", "hospital discharge"]}, {"factor": ["sex"], "outcome": ["mortality", "hospital discharge"]}, {"factor": ["glasgow coma scale score"], "outcome": ["mortality", "hospital discharge"]}]</t>
+          <t>[{"factor": ["rotterdam"], "outcome": ["hospital discharge", "mortality"]}, {"factor": ["age"], "outcome": ["hospital discharge", "mortality"]}, {"factor": ["sex"], "outcome": ["hospital discharge", "mortality"]}, {"factor": ["glasgow coma scale score"], "outcome": ["hospital discharge", "mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -2418,12 +2418,12 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>[{"factor": ["admission", "level of", "serum", "glucose"], "outcome": ["patient", "traumatic brain injury", "outcome", "severe"]}]</t>
+          <t>[{"factor": ["glucose", "serum", "admission", "level of"], "outcome": ["outcome", "traumatic brain injury", "patient", "severe"]}]</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>[{"factor": ["admission", "level of", "glucose"], "outcome": ["unspecified clinical outcome"]}]</t>
+          <t>[{"factor": ["glucose", "admission", "level of"], "outcome": ["unspecified clinical outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>[{"factor": ["il-6"], "outcome": ["favorable", "year", "gos"]}, {"factor": ["pg"], "outcome": ["favorable", "year", "gos"]}, {"factor": ["gfap"], "outcome": ["unfavorable", "year", "gos", "score"]}, {"factor": ["pg"], "outcome": ["year", "survival status"]}, {"factor": ["gfap"], "outcome": ["year", "survival status"]}, {"factor": ["il-6"], "outcome": ["year", "survival status"]}]</t>
+          <t>[{"factor": ["il-6"], "outcome": ["year", "favorable", "gos"]}, {"factor": ["pg"], "outcome": ["year", "favorable", "gos"]}, {"factor": ["gfap"], "outcome": ["unfavorable", "year", "score", "gos"]}, {"factor": ["pg"], "outcome": ["survival status", "year"]}, {"factor": ["gfap"], "outcome": ["survival status", "year"]}, {"factor": ["il-6"], "outcome": ["survival status", "year"]}]</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -2723,12 +2723,12 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>[{"factor": ["glasgow coma scale"], "outcome": ["mortality"]}, {"factor": ["mechanical ventilation"], "outcome": ["neurological"]}, {"factor": ["blood transfusion"], "outcome": ["neurological"]}, {"factor": ["neurosurgical intervention"], "outcome": ["neurological"]}, {"factor": ["concomitant", "injury"], "outcome": ["non-neurological", "complication"]}]</t>
+          <t>[{"factor": ["glasgow coma scale"], "outcome": ["mortality"]}, {"factor": ["mechanical ventilation"], "outcome": ["neurological"]}, {"factor": ["blood transfusion"], "outcome": ["neurological"]}, {"factor": ["neurosurgical intervention"], "outcome": ["neurological"]}, {"factor": ["concomitant", "injury"], "outcome": ["complication", "non-neurological"]}]</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>[{"factor": ["gcs"], "outcome": ["mortality"]}, {"factor": ["mechanical ventilation"], "outcome": ["neurological"]}, {"factor": ["blood transfusion"], "outcome": ["neurological"]}, {"factor": ["neurosurgical intervention"], "outcome": ["neurological"]}, {"factor": ["concomitant"], "outcome": ["non-neurological", "complication"]}]</t>
+          <t>[{"factor": ["gcs"], "outcome": ["mortality"]}, {"factor": ["mechanical ventilation"], "outcome": ["neurological"]}, {"factor": ["blood transfusion"], "outcome": ["neurological"]}, {"factor": ["neurosurgical intervention"], "outcome": ["neurological"]}, {"factor": ["concomitant"], "outcome": ["complication", "non-neurological"]}]</t>
         </is>
       </c>
     </row>
@@ -2784,12 +2784,12 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>[{"factor": ["traumatic brain injury"], "outcome": ["mortality"]}, {"factor": ["hospital", "refer", "systolic blood pressure"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": ["traumatic brain injury"], "outcome": ["mortality"]}, {"factor": ["hospital", "systolic blood pressure", "refer"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>[{"factor": [], "outcome": ["mortality"]}, {"factor": ["hospital", "sbp", "refer"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": [], "outcome": ["mortality"]}, {"factor": ["hospital", "refer", "sbp"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
     </row>

</xml_diff>